<commit_message>
primeira versao completa da pagina sobre, um pouco do readme e atualizacao no backlog
</commit_message>
<xml_diff>
--- a/governança/backlog-swifthub.xlsx
+++ b/governança/backlog-swifthub.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nini\Desktop\◞ ♡ ‧  ₊ ˚ faculdade\◞ ♡ 01 semestre\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nini\Desktop\◞ ♡ ‧  ₊ ˚ faculdade\◞ ♡ 01 semestre\◞ ♡ Pesquisa e inovação\Projeto Individual\SwiftHub\governança\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{577A2C09-E8F6-4E6B-8B9D-961FEF70BF45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24FA0931-83D3-4308-B19B-52392F08AEE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$1:$H$27</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="106">
   <si>
     <t>id</t>
   </si>
@@ -338,6 +337,15 @@
   </si>
   <si>
     <t>#26</t>
+  </si>
+  <si>
+    <t>VM</t>
+  </si>
+  <si>
+    <t>Instalação e configuração do ambiente dentro da maquina virtual Lubuntu</t>
+  </si>
+  <si>
+    <t>#27</t>
   </si>
 </sst>
 </file>
@@ -493,7 +501,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -553,11 +561,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="dotted">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -665,6 +682,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -963,21 +986,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="18.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.42578125" style="3" customWidth="1"/>
-    <col min="5" max="6" width="14.42578125" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" customWidth="1"/>
+    <col min="1" max="1" width="5.33203125" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.44140625" style="3" customWidth="1"/>
+    <col min="5" max="6" width="14.44140625" customWidth="1"/>
+    <col min="7" max="7" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1001,7 +1024,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" s="25" t="s">
         <v>19</v>
       </c>
@@ -1027,7 +1050,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="25" t="s">
         <v>20</v>
       </c>
@@ -1051,7 +1074,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" s="25" t="s">
         <v>21</v>
       </c>
@@ -1075,7 +1098,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5" s="25" t="s">
         <v>22</v>
       </c>
@@ -1099,7 +1122,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A6" s="25" t="s">
         <v>23</v>
       </c>
@@ -1123,7 +1146,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="25" t="s">
         <v>24</v>
       </c>
@@ -1147,7 +1170,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="25" t="s">
         <v>38</v>
       </c>
@@ -1173,7 +1196,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="25" t="s">
         <v>39</v>
       </c>
@@ -1197,7 +1220,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="25" t="s">
         <v>40</v>
       </c>
@@ -1221,7 +1244,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="25" t="s">
         <v>41</v>
       </c>
@@ -1245,7 +1268,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="25" t="s">
         <v>42</v>
       </c>
@@ -1271,7 +1294,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A13" s="25" t="s">
         <v>43</v>
       </c>
@@ -1295,7 +1318,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="25" t="s">
         <v>44</v>
       </c>
@@ -1319,7 +1342,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A15" s="25" t="s">
         <v>62</v>
       </c>
@@ -1345,7 +1368,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="25" t="s">
         <v>63</v>
       </c>
@@ -1371,7 +1394,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="25" t="s">
         <v>64</v>
       </c>
@@ -1395,7 +1418,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="25" t="s">
         <v>65</v>
       </c>
@@ -1421,7 +1444,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="25" t="s">
         <v>66</v>
       </c>
@@ -1445,7 +1468,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A20" s="25" t="s">
         <v>67</v>
       </c>
@@ -1469,7 +1492,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="25" t="s">
         <v>96</v>
       </c>
@@ -1493,7 +1516,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="25" t="s">
         <v>97</v>
       </c>
@@ -1517,7 +1540,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="25" t="s">
         <v>98</v>
       </c>
@@ -1541,7 +1564,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A24" s="25" t="s">
         <v>99</v>
       </c>
@@ -1567,7 +1590,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="25" t="s">
         <v>100</v>
       </c>
@@ -1591,7 +1614,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="25" t="s">
         <v>101</v>
       </c>
@@ -1617,7 +1640,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="25" t="s">
         <v>102</v>
       </c>
@@ -1641,17 +1664,31 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="B28" s="37" t="s">
+        <v>103</v>
+      </c>
+      <c r="C28" s="38" t="s">
+        <v>104</v>
+      </c>
+      <c r="D28" s="38"/>
+      <c r="E28" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="G28" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="H28" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1661,7 +1698,7 @@
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1671,7 +1708,7 @@
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1681,7 +1718,7 @@
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1691,7 +1728,7 @@
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1701,7 +1738,7 @@
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1715,7 +1752,8 @@
   <autoFilter ref="A1:H27" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <filterColumn colId="1" showButton="0"/>
   </autoFilter>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="C28:D28"/>
     <mergeCell ref="B26:B27"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:B7"/>

</xml_diff>